<commit_message>
index 0 as ext id and 5 as internal id for buildings import
</commit_message>
<xml_diff>
--- a/spec/files/buildings-update.xlsx
+++ b/spec/files/buildings-update.xlsx
@@ -17,7 +17,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A5">
+    <comment authorId="0" ref="F5">
       <text>
         <t xml:space="preserve">======
 ID#AAAAOnxbUpk
@@ -26,7 +26,7 @@
 _Assigned to Yogesh Mongar_</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A7">
+    <comment authorId="0" ref="F7">
       <text>
         <t xml:space="preserve">======
 ID#AAAAOgIlUVY
@@ -169,24 +169,24 @@
     <t>irrelevant</t>
   </si>
   <si>
+    <t>PROFKE</t>
+  </si>
+  <si>
+    <t>PROKAT</t>
+  </si>
+  <si>
+    <t>PROKAT string</t>
+  </si>
+  <si>
+    <t>PROPAR</t>
+  </si>
+  <si>
+    <t>PROPAR string</t>
+  </si>
+  <si>
     <t>PRONUM</t>
   </si>
   <si>
-    <t>PROKAT</t>
-  </si>
-  <si>
-    <t>PROKAT string</t>
-  </si>
-  <si>
-    <t>PROPAR</t>
-  </si>
-  <si>
-    <t>PROPAR string</t>
-  </si>
-  <si>
-    <t>PROFKE</t>
-  </si>
-  <si>
     <t>LIENUM</t>
   </si>
   <si>
@@ -367,7 +367,7 @@
     <t>RNK</t>
   </si>
   <si>
-    <t>project number</t>
+    <t>linking ID to the infomanager project</t>
   </si>
   <si>
     <t>project 
@@ -384,7 +384,7 @@
     <t>text (D)</t>
   </si>
   <si>
-    <t>linking ID to the infomanager project</t>
+    <t>project number</t>
   </si>
   <si>
     <t>buidling 
@@ -1780,7 +1780,7 @@
     <font/>
     <font>
       <color rgb="FF74A4C8"/>
-      <name val="&quot;JetBrains Mono&quot;"/>
+      <name val="JetBrains Mono"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -1789,7 +1789,7 @@
     </font>
     <font>
       <color rgb="FF6A8759"/>
-      <name val="&quot;JetBrains Mono&quot;"/>
+      <name val="JetBrains Mono"/>
     </font>
     <font>
       <u/>
@@ -1906,26 +1906,20 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -2239,9 +2233,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.38"/>
+    <col customWidth="1" min="1" max="1" width="22.5"/>
     <col customWidth="1" min="2" max="5" width="8.25"/>
-    <col customWidth="1" min="6" max="6" width="22.5"/>
+    <col customWidth="1" min="6" max="6" width="10.38"/>
     <col customWidth="1" min="7" max="7" width="13.88"/>
     <col customWidth="1" min="8" max="13" width="16.25"/>
     <col customWidth="1" min="14" max="14" width="8.25"/>
@@ -2267,14 +2261,14 @@
   </cols>
   <sheetData>
     <row r="1" ht="33.0" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -2403,9 +2397,7 @@
       <c r="BN1" s="1"/>
     </row>
     <row r="2" ht="38.25" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
@@ -2418,7 +2410,9 @@
       <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2932,204 +2926,204 @@
       <c r="A6" s="6">
         <v>0.0</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>1.0</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>2.0</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="7">
         <v>3.0</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="7">
         <v>4.0</v>
       </c>
       <c r="F6" s="6">
         <v>5.0</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="7">
         <v>6.0</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="7">
         <v>7.0</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="7">
         <v>8.0</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="7">
         <v>9.0</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="7">
         <v>10.0</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="7">
         <v>11.0</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="7">
         <v>12.0</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="7">
         <v>13.0</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="7">
         <v>14.0</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="7">
         <v>15.0</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="7">
         <v>16.0</v>
       </c>
-      <c r="R6" s="6">
+      <c r="R6" s="7">
         <v>17.0</v>
       </c>
-      <c r="S6" s="6">
+      <c r="S6" s="7">
         <v>18.0</v>
       </c>
-      <c r="T6" s="6">
+      <c r="T6" s="7">
         <v>19.0</v>
       </c>
-      <c r="U6" s="6">
+      <c r="U6" s="7">
         <v>20.0</v>
       </c>
-      <c r="V6" s="6">
+      <c r="V6" s="7">
         <v>21.0</v>
       </c>
-      <c r="W6" s="6">
+      <c r="W6" s="7">
         <v>22.0</v>
       </c>
-      <c r="X6" s="6">
+      <c r="X6" s="7">
         <v>23.0</v>
       </c>
-      <c r="Y6" s="6">
+      <c r="Y6" s="7">
         <v>24.0</v>
       </c>
-      <c r="Z6" s="6">
+      <c r="Z6" s="7">
         <v>25.0</v>
       </c>
-      <c r="AA6" s="6">
+      <c r="AA6" s="7">
         <v>26.0</v>
       </c>
-      <c r="AB6" s="6">
+      <c r="AB6" s="7">
         <v>27.0</v>
       </c>
-      <c r="AC6" s="6">
+      <c r="AC6" s="7">
         <v>28.0</v>
       </c>
-      <c r="AD6" s="6">
+      <c r="AD6" s="7">
         <v>29.0</v>
       </c>
-      <c r="AE6" s="6">
+      <c r="AE6" s="7">
         <v>30.0</v>
       </c>
-      <c r="AF6" s="6">
+      <c r="AF6" s="7">
         <v>31.0</v>
       </c>
-      <c r="AG6" s="6">
+      <c r="AG6" s="7">
         <v>32.0</v>
       </c>
-      <c r="AH6" s="6">
+      <c r="AH6" s="7">
         <v>33.0</v>
       </c>
-      <c r="AI6" s="6">
+      <c r="AI6" s="7">
         <v>34.0</v>
       </c>
-      <c r="AJ6" s="6">
+      <c r="AJ6" s="7">
         <v>35.0</v>
       </c>
-      <c r="AK6" s="6">
+      <c r="AK6" s="7">
         <v>36.0</v>
       </c>
-      <c r="AL6" s="6">
+      <c r="AL6" s="7">
         <v>37.0</v>
       </c>
-      <c r="AM6" s="6">
+      <c r="AM6" s="7">
         <v>38.0</v>
       </c>
-      <c r="AN6" s="6">
+      <c r="AN6" s="7">
         <v>39.0</v>
       </c>
-      <c r="AO6" s="6">
+      <c r="AO6" s="7">
         <v>40.0</v>
       </c>
-      <c r="AP6" s="6">
+      <c r="AP6" s="7">
         <v>41.0</v>
       </c>
-      <c r="AQ6" s="6">
+      <c r="AQ6" s="7">
         <v>42.0</v>
       </c>
-      <c r="AR6" s="6">
+      <c r="AR6" s="7">
         <v>43.0</v>
       </c>
-      <c r="AS6" s="6">
+      <c r="AS6" s="7">
         <v>44.0</v>
       </c>
-      <c r="AT6" s="6">
+      <c r="AT6" s="7">
         <v>45.0</v>
       </c>
-      <c r="AU6" s="6">
+      <c r="AU6" s="7">
         <v>46.0</v>
       </c>
-      <c r="AV6" s="6">
+      <c r="AV6" s="7">
         <v>47.0</v>
       </c>
-      <c r="AW6" s="6">
+      <c r="AW6" s="7">
         <v>48.0</v>
       </c>
-      <c r="AX6" s="6">
+      <c r="AX6" s="7">
         <v>49.0</v>
       </c>
-      <c r="AY6" s="6">
+      <c r="AY6" s="7">
         <v>50.0</v>
       </c>
-      <c r="AZ6" s="6">
+      <c r="AZ6" s="7">
         <v>51.0</v>
       </c>
-      <c r="BA6" s="6">
+      <c r="BA6" s="7">
         <v>52.0</v>
       </c>
-      <c r="BB6" s="6">
+      <c r="BB6" s="7">
         <v>53.0</v>
       </c>
-      <c r="BC6" s="6">
+      <c r="BC6" s="7">
         <v>54.0</v>
       </c>
-      <c r="BD6" s="6">
+      <c r="BD6" s="7">
         <v>55.0</v>
       </c>
-      <c r="BE6" s="6">
+      <c r="BE6" s="7">
         <v>56.0</v>
       </c>
-      <c r="BF6" s="6">
+      <c r="BF6" s="7">
         <v>57.0</v>
       </c>
-      <c r="BG6" s="6">
+      <c r="BG6" s="7">
         <v>58.0</v>
       </c>
-      <c r="BH6" s="6">
+      <c r="BH6" s="7">
         <v>59.0</v>
       </c>
-      <c r="BI6" s="6">
+      <c r="BI6" s="7">
         <v>60.0</v>
       </c>
-      <c r="BJ6" s="6">
+      <c r="BJ6" s="7">
         <v>61.0</v>
       </c>
-      <c r="BK6" s="6">
+      <c r="BK6" s="7">
         <v>62.0</v>
       </c>
-      <c r="BL6" s="6">
+      <c r="BL6" s="7">
         <v>63.0</v>
       </c>
-      <c r="BM6" s="6">
+      <c r="BM6" s="7">
         <v>64.0</v>
       </c>
-      <c r="BN6" s="6">
+      <c r="BN6" s="7">
         <v>65.0</v>
       </c>
     </row>
     <row r="7" ht="62.25" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -3144,7 +3138,7 @@
       <c r="E7" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>103</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -3329,7 +3323,9 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8">
+        <v>3017545.0</v>
+      </c>
       <c r="B8" s="5">
         <v>3892.0</v>
       </c>
@@ -3342,9 +3338,7 @@
       <c r="E8" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F8" s="8">
-        <v>3017545.0</v>
-      </c>
+      <c r="F8" s="5"/>
       <c r="G8" s="9">
         <v>58580.0</v>
       </c>
@@ -3483,7 +3477,9 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8">
+        <v>3017545.0</v>
+      </c>
       <c r="B9" s="5">
         <v>3892.0</v>
       </c>
@@ -3496,9 +3492,7 @@
       <c r="E9" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F9" s="8">
-        <v>3017545.0</v>
-      </c>
+      <c r="F9" s="5"/>
       <c r="G9" s="9">
         <v>58581.0</v>
       </c>
@@ -3635,7 +3629,9 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8">
+        <v>3017545.0</v>
+      </c>
       <c r="B10" s="5">
         <v>3892.0</v>
       </c>
@@ -3648,9 +3644,7 @@
       <c r="E10" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="8">
-        <v>3017545.0</v>
-      </c>
+      <c r="F10" s="5"/>
       <c r="G10" s="13">
         <v>8.295225E7</v>
       </c>
@@ -3787,9 +3781,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="14">
-        <v>312583.0</v>
-      </c>
+      <c r="A11" s="8"/>
       <c r="B11" s="5">
         <v>3892.0</v>
       </c>
@@ -3802,7 +3794,9 @@
       <c r="E11" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="14">
+        <v>312583.0</v>
+      </c>
       <c r="G11" s="13">
         <v>8.2952247E7</v>
       </c>
@@ -3939,9 +3933,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="14">
-        <v>312583.0</v>
-      </c>
+      <c r="A12" s="8"/>
       <c r="B12" s="5">
         <v>3892.0</v>
       </c>
@@ -3954,7 +3946,9 @@
       <c r="E12" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="14">
+        <v>312583.0</v>
+      </c>
       <c r="G12" s="13">
         <v>8.2952235E7</v>
       </c>
@@ -4089,9 +4083,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="14">
-        <v>312583.0</v>
-      </c>
+      <c r="A13" s="8"/>
       <c r="B13" s="5">
         <v>3892.0</v>
       </c>
@@ -4104,7 +4096,9 @@
       <c r="E13" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="14">
+        <v>312583.0</v>
+      </c>
       <c r="G13" s="13">
         <v>8.2952236E7</v>
       </c>
@@ -4241,8 +4235,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="14">
-        <v>312583.0</v>
+      <c r="A14" s="8">
+        <v>3017545.0</v>
       </c>
       <c r="B14" s="5">
         <v>3892.0</v>
@@ -4256,8 +4250,8 @@
       <c r="E14" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F14" s="8">
-        <v>3017545.0</v>
+      <c r="F14" s="14">
+        <v>312583.0</v>
       </c>
       <c r="G14" s="5">
         <v>8.2952237E7</v>
@@ -4391,8 +4385,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7">
-        <v>312584.0</v>
+      <c r="A15" s="5">
+        <v>653818.0</v>
       </c>
       <c r="B15" s="5">
         <v>3892.0</v>
@@ -4407,7 +4401,7 @@
         <v>157</v>
       </c>
       <c r="F15" s="5">
-        <v>653818.0</v>
+        <v>312584.0</v>
       </c>
       <c r="G15" s="5">
         <v>8.2952238E7</v>
@@ -4541,8 +4535,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="7">
-        <v>312584.0</v>
+      <c r="A16" s="5">
+        <v>653818.0</v>
       </c>
       <c r="B16" s="5">
         <v>3892.0</v>
@@ -4557,7 +4551,7 @@
         <v>157</v>
       </c>
       <c r="F16" s="5">
-        <v>653818.0</v>
+        <v>312584.0</v>
       </c>
       <c r="G16" s="5">
         <v>8.2952239E7</v>
@@ -4691,8 +4685,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="7">
-        <v>312584.0</v>
+      <c r="A17" s="5">
+        <v>653818.0</v>
       </c>
       <c r="B17" s="5">
         <v>3892.0</v>
@@ -4707,7 +4701,7 @@
         <v>157</v>
       </c>
       <c r="F17" s="5">
-        <v>653818.0</v>
+        <v>312584.0</v>
       </c>
       <c r="G17" s="5">
         <v>8.295224E7</v>
@@ -4845,8 +4839,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="7">
-        <v>312584.0</v>
+      <c r="A18" s="5">
+        <v>653818.0</v>
       </c>
       <c r="B18" s="5">
         <v>3892.0</v>
@@ -4861,7 +4855,7 @@
         <v>157</v>
       </c>
       <c r="F18" s="5">
-        <v>653818.0</v>
+        <v>312584.0</v>
       </c>
       <c r="G18" s="5">
         <v>8.2952241E7</v>
@@ -4999,8 +4993,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="7">
-        <v>312584.0</v>
+      <c r="A19" s="5">
+        <v>653818.0</v>
       </c>
       <c r="B19" s="5">
         <v>3892.0</v>
@@ -5015,7 +5009,7 @@
         <v>157</v>
       </c>
       <c r="F19" s="5">
-        <v>653818.0</v>
+        <v>312584.0</v>
       </c>
       <c r="G19" s="5">
         <v>8.2952242E7</v>
@@ -5153,8 +5147,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="7">
-        <v>312584.0</v>
+      <c r="A20" s="5">
+        <v>653818.0</v>
       </c>
       <c r="B20" s="5">
         <v>3892.0</v>
@@ -5169,7 +5163,7 @@
         <v>157</v>
       </c>
       <c r="F20" s="5">
-        <v>653818.0</v>
+        <v>312584.0</v>
       </c>
       <c r="G20" s="5">
         <v>8.2952243E7</v>
@@ -5307,8 +5301,8 @@
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="7">
-        <v>312584.0</v>
+      <c r="A21" s="5">
+        <v>653818.0</v>
       </c>
       <c r="B21" s="5">
         <v>3892.0</v>
@@ -5323,7 +5317,7 @@
         <v>157</v>
       </c>
       <c r="F21" s="5">
-        <v>653818.0</v>
+        <v>312584.0</v>
       </c>
       <c r="G21" s="5">
         <v>8.2952244E7</v>
@@ -5462,7 +5456,7 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="5">
-        <v>312579.0</v>
+        <v>752643.0</v>
       </c>
       <c r="B22" s="5">
         <v>3892.0</v>
@@ -5477,7 +5471,7 @@
         <v>157</v>
       </c>
       <c r="F22" s="5">
-        <v>752643.0</v>
+        <v>312579.0</v>
       </c>
       <c r="G22" s="5">
         <v>8.295223E7</v>
@@ -5616,7 +5610,7 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="5">
-        <v>312579.0</v>
+        <v>752643.0</v>
       </c>
       <c r="B23" s="5">
         <v>3892.0</v>
@@ -5631,7 +5625,7 @@
         <v>157</v>
       </c>
       <c r="F23" s="5">
-        <v>752643.0</v>
+        <v>312579.0</v>
       </c>
       <c r="G23" s="5">
         <v>8.2952231E7</v>
@@ -5770,7 +5764,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="5">
-        <v>312578.0</v>
+        <v>755762.0</v>
       </c>
       <c r="B24" s="5">
         <v>3892.0</v>
@@ -5785,7 +5779,7 @@
         <v>157</v>
       </c>
       <c r="F24" s="5">
-        <v>755762.0</v>
+        <v>312578.0</v>
       </c>
       <c r="G24" s="5">
         <v>8.2952229E7</v>
@@ -5922,7 +5916,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="5">
-        <v>312577.0</v>
+        <v>740883.0</v>
       </c>
       <c r="B25" s="5">
         <v>3892.0</v>
@@ -5937,7 +5931,7 @@
         <v>157</v>
       </c>
       <c r="F25" s="5">
-        <v>740883.0</v>
+        <v>312577.0</v>
       </c>
       <c r="G25" s="5">
         <v>8.2952228E7</v>
@@ -6074,7 +6068,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="5">
-        <v>312576.0</v>
+        <v>711202.0</v>
       </c>
       <c r="B26" s="5">
         <v>3892.0</v>
@@ -6089,7 +6083,7 @@
         <v>157</v>
       </c>
       <c r="F26" s="5">
-        <v>711202.0</v>
+        <v>312576.0</v>
       </c>
       <c r="G26" s="5">
         <v>8.2952227E7</v>
@@ -6226,7 +6220,7 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="5">
-        <v>312575.0</v>
+        <v>744843.0</v>
       </c>
       <c r="B27" s="5">
         <v>3892.0</v>
@@ -6241,7 +6235,7 @@
         <v>157</v>
       </c>
       <c r="F27" s="5">
-        <v>744843.0</v>
+        <v>312575.0</v>
       </c>
       <c r="G27" s="5">
         <v>8.2952226E7</v>
@@ -6378,7 +6372,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="5">
-        <v>312573.0</v>
+        <v>758655.0</v>
       </c>
       <c r="B28" s="5">
         <v>3892.0</v>
@@ -6393,7 +6387,7 @@
         <v>157</v>
       </c>
       <c r="F28" s="5">
-        <v>758655.0</v>
+        <v>312573.0</v>
       </c>
       <c r="G28" s="5">
         <v>8.2952222E7</v>
@@ -6532,7 +6526,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="5">
-        <v>312573.0</v>
+        <v>758655.0</v>
       </c>
       <c r="B29" s="5">
         <v>3892.0</v>
@@ -6547,7 +6541,7 @@
         <v>157</v>
       </c>
       <c r="F29" s="5">
-        <v>758655.0</v>
+        <v>312573.0</v>
       </c>
       <c r="G29" s="5">
         <v>8.2952223E7</v>
@@ -6686,7 +6680,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="5">
-        <v>312573.0</v>
+        <v>758655.0</v>
       </c>
       <c r="B30" s="5">
         <v>3892.0</v>
@@ -6701,7 +6695,7 @@
         <v>157</v>
       </c>
       <c r="F30" s="5">
-        <v>758655.0</v>
+        <v>312573.0</v>
       </c>
       <c r="G30" s="5">
         <v>8.2952224E7</v>
@@ -6838,7 +6832,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="5">
-        <v>312572.0</v>
+        <v>764282.0</v>
       </c>
       <c r="B31" s="5">
         <v>3892.0</v>
@@ -6853,7 +6847,7 @@
         <v>157</v>
       </c>
       <c r="F31" s="5">
-        <v>764282.0</v>
+        <v>312572.0</v>
       </c>
       <c r="G31" s="5">
         <v>8.2951643E7</v>
@@ -6990,7 +6984,7 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="5">
-        <v>312571.0</v>
+        <v>510842.0</v>
       </c>
       <c r="B32" s="5">
         <v>3892.0</v>
@@ -7005,7 +6999,7 @@
         <v>157</v>
       </c>
       <c r="F32" s="5">
-        <v>510842.0</v>
+        <v>312571.0</v>
       </c>
       <c r="G32" s="5">
         <v>8.2951642E7</v>
@@ -7146,7 +7140,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="5">
-        <v>309913.0</v>
+        <v>706904.0</v>
       </c>
       <c r="B33" s="5">
         <v>3892.0</v>
@@ -7161,7 +7155,7 @@
         <v>157</v>
       </c>
       <c r="F33" s="5">
-        <v>706904.0</v>
+        <v>309913.0</v>
       </c>
       <c r="G33" s="5">
         <v>8.290936E7</v>
@@ -7310,7 +7304,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="5">
-        <v>309913.0</v>
+        <v>706904.0</v>
       </c>
       <c r="B34" s="5">
         <v>3892.0</v>
@@ -7325,7 +7319,7 @@
         <v>157</v>
       </c>
       <c r="F34" s="5">
-        <v>706904.0</v>
+        <v>309913.0</v>
       </c>
       <c r="G34" s="5">
         <v>8.2909361E7</v>
@@ -7474,7 +7468,7 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="5">
-        <v>309913.0</v>
+        <v>706904.0</v>
       </c>
       <c r="B35" s="5">
         <v>3892.0</v>
@@ -7489,7 +7483,7 @@
         <v>157</v>
       </c>
       <c r="F35" s="5">
-        <v>706904.0</v>
+        <v>309913.0</v>
       </c>
       <c r="G35" s="5">
         <v>8.2909362E7</v>
@@ -7638,7 +7632,7 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="5">
-        <v>309913.0</v>
+        <v>706904.0</v>
       </c>
       <c r="B36" s="5">
         <v>3892.0</v>
@@ -7653,7 +7647,7 @@
         <v>157</v>
       </c>
       <c r="F36" s="5">
-        <v>706904.0</v>
+        <v>309913.0</v>
       </c>
       <c r="G36" s="5">
         <v>8.2909363E7</v>
@@ -7802,7 +7796,7 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="5">
-        <v>309913.0</v>
+        <v>706904.0</v>
       </c>
       <c r="B37" s="5">
         <v>3892.0</v>
@@ -7817,7 +7811,7 @@
         <v>157</v>
       </c>
       <c r="F37" s="5">
-        <v>706904.0</v>
+        <v>309913.0</v>
       </c>
       <c r="G37" s="5">
         <v>8.2909364E7</v>
@@ -7966,7 +7960,7 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="5">
-        <v>309913.0</v>
+        <v>706904.0</v>
       </c>
       <c r="B38" s="5">
         <v>3892.0</v>
@@ -7981,7 +7975,7 @@
         <v>157</v>
       </c>
       <c r="F38" s="5">
-        <v>706904.0</v>
+        <v>309913.0</v>
       </c>
       <c r="G38" s="5">
         <v>8.2909365E7</v>
@@ -8130,7 +8124,7 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="5">
-        <v>312561.0</v>
+        <v>699422.0</v>
       </c>
       <c r="B39" s="5">
         <v>3892.0</v>
@@ -8145,7 +8139,7 @@
         <v>157</v>
       </c>
       <c r="F39" s="5">
-        <v>699422.0</v>
+        <v>312561.0</v>
       </c>
       <c r="G39" s="5">
         <v>8.2951609E7</v>
@@ -8282,7 +8276,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="5">
-        <v>312561.0</v>
+        <v>699422.0</v>
       </c>
       <c r="B40" s="5">
         <v>3892.0</v>
@@ -8297,7 +8291,7 @@
         <v>157</v>
       </c>
       <c r="F40" s="5">
-        <v>699422.0</v>
+        <v>312561.0</v>
       </c>
       <c r="G40" s="5">
         <v>8.295161E7</v>
@@ -8434,7 +8428,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="5">
-        <v>312560.0</v>
+        <v>732509.0</v>
       </c>
       <c r="B41" s="5">
         <v>3892.0</v>
@@ -8449,7 +8443,7 @@
         <v>157</v>
       </c>
       <c r="F41" s="5">
-        <v>732509.0</v>
+        <v>312560.0</v>
       </c>
       <c r="G41" s="5">
         <v>8.2951608E7</v>
@@ -8588,7 +8582,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="5">
-        <v>312558.0</v>
+        <v>758038.0</v>
       </c>
       <c r="B42" s="5">
         <v>3892.0</v>
@@ -8603,7 +8597,7 @@
         <v>157</v>
       </c>
       <c r="F42" s="5">
-        <v>758038.0</v>
+        <v>312558.0</v>
       </c>
       <c r="G42" s="5">
         <v>8.29516E7</v>
@@ -8740,7 +8734,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="5">
-        <v>312551.0</v>
+        <v>647649.0</v>
       </c>
       <c r="B43" s="5">
         <v>3892.0</v>
@@ -8755,7 +8749,7 @@
         <v>157</v>
       </c>
       <c r="F43" s="5">
-        <v>647649.0</v>
+        <v>312551.0</v>
       </c>
       <c r="G43" s="5">
         <v>8.2951588E7</v>
@@ -8892,7 +8886,7 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="5">
-        <v>312551.0</v>
+        <v>647649.0</v>
       </c>
       <c r="B44" s="5">
         <v>3892.0</v>
@@ -8907,7 +8901,7 @@
         <v>157</v>
       </c>
       <c r="F44" s="5">
-        <v>647649.0</v>
+        <v>312551.0</v>
       </c>
       <c r="G44" s="5">
         <v>8.2951589E7</v>
@@ -9044,7 +9038,7 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="5">
-        <v>310754.0</v>
+        <v>723768.0</v>
       </c>
       <c r="B45" s="5">
         <v>3892.0</v>
@@ -9059,7 +9053,7 @@
         <v>157</v>
       </c>
       <c r="F45" s="5">
-        <v>723768.0</v>
+        <v>310754.0</v>
       </c>
       <c r="G45" s="5">
         <v>8.292038E7</v>
@@ -9216,7 +9210,7 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="5">
-        <v>312017.0</v>
+        <v>750363.0</v>
       </c>
       <c r="B46" s="5">
         <v>3892.0</v>
@@ -9231,7 +9225,7 @@
         <v>157</v>
       </c>
       <c r="F46" s="5">
-        <v>750363.0</v>
+        <v>312017.0</v>
       </c>
       <c r="G46" s="5">
         <v>8.2944528E7</v>
@@ -9368,7 +9362,7 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="5">
-        <v>305403.0</v>
+        <v>637800.0</v>
       </c>
       <c r="B47" s="5">
         <v>3892.0</v>
@@ -9383,7 +9377,7 @@
         <v>157</v>
       </c>
       <c r="F47" s="5">
-        <v>637800.0</v>
+        <v>305403.0</v>
       </c>
       <c r="G47" s="5">
         <v>8.275556E7</v>
@@ -9542,7 +9536,7 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="5">
-        <v>310834.0</v>
+        <v>56073.0</v>
       </c>
       <c r="B48" s="5">
         <v>13272.0</v>
@@ -9557,7 +9551,7 @@
         <v>157</v>
       </c>
       <c r="F48" s="5">
-        <v>56073.0</v>
+        <v>310834.0</v>
       </c>
       <c r="G48" s="5">
         <v>8.2920494E7</v>
@@ -9714,7 +9708,7 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="5">
-        <v>311122.0</v>
+        <v>479563.0</v>
       </c>
       <c r="B49" s="5">
         <v>3892.0</v>
@@ -9729,7 +9723,7 @@
         <v>157</v>
       </c>
       <c r="F49" s="5">
-        <v>479563.0</v>
+        <v>311122.0</v>
       </c>
       <c r="G49" s="5">
         <v>8.2926926E7</v>
@@ -9892,7 +9886,7 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="5">
-        <v>306387.0</v>
+        <v>663832.0</v>
       </c>
       <c r="B50" s="5">
         <v>3892.0</v>
@@ -9907,7 +9901,7 @@
         <v>157</v>
       </c>
       <c r="F50" s="5">
-        <v>663832.0</v>
+        <v>306387.0</v>
       </c>
       <c r="G50" s="5">
         <v>8.2760258E7</v>
@@ -10074,7 +10068,7 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="5">
-        <v>309674.0</v>
+        <v>705796.0</v>
       </c>
       <c r="B51" s="5">
         <v>3892.0</v>
@@ -10089,7 +10083,7 @@
         <v>157</v>
       </c>
       <c r="F51" s="5">
-        <v>705796.0</v>
+        <v>309674.0</v>
       </c>
       <c r="G51" s="5">
         <v>8.2908096E7</v>
@@ -10252,7 +10246,7 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="5">
-        <v>310867.0</v>
+        <v>719589.0</v>
       </c>
       <c r="B52" s="5">
         <v>3892.0</v>
@@ -10267,7 +10261,7 @@
         <v>157</v>
       </c>
       <c r="F52" s="5">
-        <v>719589.0</v>
+        <v>310867.0</v>
       </c>
       <c r="G52" s="5">
         <v>8.2921551E7</v>
@@ -10430,7 +10424,7 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="5">
-        <v>310586.0</v>
+        <v>725725.0</v>
       </c>
       <c r="B53" s="5">
         <v>3892.0</v>
@@ -10445,7 +10439,7 @@
         <v>157</v>
       </c>
       <c r="F53" s="5">
-        <v>725725.0</v>
+        <v>310586.0</v>
       </c>
       <c r="G53" s="5">
         <v>8.2916998E7</v>
@@ -10608,7 +10602,7 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="5">
-        <v>310536.0</v>
+        <v>714128.0</v>
       </c>
       <c r="B54" s="5">
         <v>3892.0</v>
@@ -10623,7 +10617,7 @@
         <v>157</v>
       </c>
       <c r="F54" s="5">
-        <v>714128.0</v>
+        <v>310536.0</v>
       </c>
       <c r="G54" s="5">
         <v>8.2916919E7</v>
@@ -10786,7 +10780,7 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="5">
-        <v>309950.0</v>
+        <v>624081.0</v>
       </c>
       <c r="B55" s="5">
         <v>3892.0</v>
@@ -10801,7 +10795,7 @@
         <v>157</v>
       </c>
       <c r="F55" s="5">
-        <v>624081.0</v>
+        <v>309950.0</v>
       </c>
       <c r="G55" s="5">
         <v>8.2909437E7</v>
@@ -10962,7 +10956,7 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="5">
-        <v>312545.0</v>
+        <v>743814.0</v>
       </c>
       <c r="B56" s="5">
         <v>3892.0</v>
@@ -10977,7 +10971,7 @@
         <v>157</v>
       </c>
       <c r="F56" s="5">
-        <v>743814.0</v>
+        <v>312545.0</v>
       </c>
       <c r="G56" s="5">
         <v>8.2951566E7</v>
@@ -11132,7 +11126,7 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="5">
-        <v>301188.0</v>
+        <v>582760.0</v>
       </c>
       <c r="B57" s="5">
         <v>3892.0</v>
@@ -11147,7 +11141,7 @@
         <v>157</v>
       </c>
       <c r="F57" s="5">
-        <v>582760.0</v>
+        <v>301188.0</v>
       </c>
       <c r="G57" s="5">
         <v>8.2735245E7</v>
@@ -11306,7 +11300,7 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="5">
-        <v>301188.0</v>
+        <v>582760.0</v>
       </c>
       <c r="B58" s="5">
         <v>3892.0</v>
@@ -11321,7 +11315,7 @@
         <v>157</v>
       </c>
       <c r="F58" s="5">
-        <v>582760.0</v>
+        <v>301188.0</v>
       </c>
       <c r="G58" s="5">
         <v>8.2735246E7</v>
@@ -11480,7 +11474,7 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="5">
-        <v>301188.0</v>
+        <v>582760.0</v>
       </c>
       <c r="B59" s="5">
         <v>3892.0</v>
@@ -11495,7 +11489,7 @@
         <v>157</v>
       </c>
       <c r="F59" s="5">
-        <v>582760.0</v>
+        <v>301188.0</v>
       </c>
       <c r="G59" s="5">
         <v>8.2735247E7</v>
@@ -11654,7 +11648,7 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="5">
-        <v>301188.0</v>
+        <v>582760.0</v>
       </c>
       <c r="B60" s="5">
         <v>3892.0</v>
@@ -11669,7 +11663,7 @@
         <v>157</v>
       </c>
       <c r="F60" s="5">
-        <v>582760.0</v>
+        <v>301188.0</v>
       </c>
       <c r="G60" s="5">
         <v>8.2735248E7</v>
@@ -11828,7 +11822,7 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="5">
-        <v>301188.0</v>
+        <v>582760.0</v>
       </c>
       <c r="B61" s="5">
         <v>3892.0</v>
@@ -11843,7 +11837,7 @@
         <v>157</v>
       </c>
       <c r="F61" s="5">
-        <v>582760.0</v>
+        <v>301188.0</v>
       </c>
       <c r="G61" s="5">
         <v>8.2735249E7</v>
@@ -12002,7 +11996,7 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="5">
-        <v>301188.0</v>
+        <v>582760.0</v>
       </c>
       <c r="B62" s="5">
         <v>3892.0</v>
@@ -12017,7 +12011,7 @@
         <v>157</v>
       </c>
       <c r="F62" s="5">
-        <v>582760.0</v>
+        <v>301188.0</v>
       </c>
       <c r="G62" s="5">
         <v>8.273525E7</v>
@@ -12176,7 +12170,7 @@
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="5">
-        <v>308387.0</v>
+        <v>691005.0</v>
       </c>
       <c r="B63" s="5">
         <v>3892.0</v>
@@ -12191,7 +12185,7 @@
         <v>157</v>
       </c>
       <c r="F63" s="5">
-        <v>691005.0</v>
+        <v>308387.0</v>
       </c>
       <c r="G63" s="5">
         <v>8.2771684E7</v>
@@ -12354,7 +12348,7 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="5">
-        <v>312480.0</v>
+        <v>742071.0</v>
       </c>
       <c r="B64" s="5">
         <v>3892.0</v>
@@ -12369,7 +12363,7 @@
         <v>157</v>
       </c>
       <c r="F64" s="5">
-        <v>742071.0</v>
+        <v>312480.0</v>
       </c>
       <c r="G64" s="5">
         <v>8.2949175E7</v>
@@ -12524,7 +12518,7 @@
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="5">
-        <v>312302.0</v>
+        <v>747387.0</v>
       </c>
       <c r="B65" s="5">
         <v>3892.0</v>
@@ -12539,7 +12533,7 @@
         <v>157</v>
       </c>
       <c r="F65" s="5">
-        <v>747387.0</v>
+        <v>312302.0</v>
       </c>
       <c r="G65" s="5">
         <v>8.2947069E7</v>
@@ -12694,7 +12688,7 @@
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="5">
-        <v>312301.0</v>
+        <v>750960.0</v>
       </c>
       <c r="B66" s="5">
         <v>3892.0</v>
@@ -12709,7 +12703,7 @@
         <v>157</v>
       </c>
       <c r="F66" s="5">
-        <v>750960.0</v>
+        <v>312301.0</v>
       </c>
       <c r="G66" s="5">
         <v>8.2947068E7</v>
@@ -15429,7 +15423,7 @@
         <v>36</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G2" s="25" t="s">
         <v>38</v>

</xml_diff>